<commit_message>
notask: init sa radar
</commit_message>
<xml_diff>
--- a/public/techRadarSourceSa.xlsx
+++ b/public/techRadarSourceSa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\tech-radar\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfa/web-alfa/tech-radar/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39434DE-4395-4F3C-9B7D-CEE02D7D2BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97810AA-4432-AF40-8284-65DCEAA141A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{D0E5AF86-51E4-4329-BFCB-5FE4200F8556}"/>
+    <workbookView xWindow="2080" yWindow="1400" windowWidth="34560" windowHeight="15720" xr2:uid="{D0E5AF86-51E4-4329-BFCB-5FE4200F8556}"/>
   </bookViews>
   <sheets>
     <sheet name="radar" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="125">
   <si>
     <t>Ноль</t>
   </si>
@@ -75,12 +75,6 @@
     <t>swagger</t>
   </si>
   <si>
-    <t>microfrontends</t>
-  </si>
-  <si>
-    <t>modulefederation</t>
-  </si>
-  <si>
     <t>Strapi</t>
   </si>
   <si>
@@ -90,24 +84,15 @@
     <t>lighthouse</t>
   </si>
   <si>
-    <t>openspec first</t>
-  </si>
-  <si>
     <t>drawio</t>
   </si>
   <si>
-    <t>markdown</t>
-  </si>
-  <si>
     <t>websocket</t>
   </si>
   <si>
     <t>SSE</t>
   </si>
   <si>
-    <t>docker</t>
-  </si>
-  <si>
     <t>cursor</t>
   </si>
   <si>
@@ -180,9 +165,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>kubernetes</t>
-  </si>
-  <si>
     <t>https://www.npmjs.com/package/chatgpt</t>
   </si>
   <si>
@@ -192,24 +174,12 @@
     <t>https://www.npmjs.com/package/gemini</t>
   </si>
   <si>
-    <t>https://www.npmjs.com/package/openspec first</t>
-  </si>
-  <si>
-    <t>https://www.npmjs.com/package/microfrontends</t>
-  </si>
-  <si>
-    <t>https://www.npmjs.com/package/modulefederation</t>
-  </si>
-  <si>
     <t>https://www.npmjs.com/package/drawio</t>
   </si>
   <si>
     <t>https://www.npmjs.com/package/dynosareus</t>
   </si>
   <si>
-    <t>https://www.npmjs.com/package/markdown</t>
-  </si>
-  <si>
     <t>https://www.npmjs.com/package/typedoc</t>
   </si>
   <si>
@@ -234,12 +204,6 @@
     <t>https://www.npmjs.com/package/pluntuml</t>
   </si>
   <si>
-    <t>https://www.npmjs.com/package/docker</t>
-  </si>
-  <si>
-    <t>https://www.npmjs.com/package/kubernetes</t>
-  </si>
-  <si>
     <t>ChatGPT is OpenAI’s large‑language‑model API providing text and multimodal generation capabilities.</t>
   </si>
   <si>
@@ -249,15 +213,6 @@
     <t>Gemini is Google’s multimodal LLM platform providing text, vision, and code generation APIs.</t>
   </si>
   <si>
-    <t>Technology description from official documentation is not yet defined.</t>
-  </si>
-  <si>
-    <t>Microfrontends is an architectural style where the UI is split into independently deployable frontend modules.</t>
-  </si>
-  <si>
-    <t>Webpack Module Federation enables runtime code sharing between separately built JavaScript bundles.</t>
-  </si>
-  <si>
     <t>MUI is a React component library implementing Material Design system components.</t>
   </si>
   <si>
@@ -267,12 +222,6 @@
     <t>plantuml (likely pluntuml) renders UML diagrams from plain‑text descriptions.</t>
   </si>
   <si>
-    <t>Docker is a containerization platform for packaging applications and dependencies into portable containers.</t>
-  </si>
-  <si>
-    <t>Kubernetes is an orchestration platform for deploying, scaling, and managing containerized applications.</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -315,9 +264,6 @@
     <t>REST как архитектурный стиль — это способ проектирования API, основанный на HTTP-методах и ресурсах (нет конкретного npm-пакета под это имя).</t>
   </si>
   <si>
-    <t>rest</t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
@@ -346,6 +292,130 @@
   </si>
   <si>
     <t>Frameworks</t>
+  </si>
+  <si>
+    <t>Patterns</t>
+  </si>
+  <si>
+    <t>Contract-First (API-First)</t>
+  </si>
+  <si>
+    <t>https://swagger.io/resources/articles/adopting-an-api-first-approach/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">API-first подход в разработке программного обеспечения — это стратегия, при которой проектирование и создание программных интерфейсов (API) происходит на начальной стадии разработки, прежде чем будут реализованы другие компоненты системы. </t>
+  </si>
+  <si>
+    <t>REST API</t>
+  </si>
+  <si>
+    <t>AlfaGen</t>
+  </si>
+  <si>
+    <t>https://confluence.moscow.alfaintra.net/pages/viewpage.action?pageId=1473671047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AlfaGen -  это платформа, разработанная в Банке, которая позволяет создавать новые клиентские пути и новый UX для продуктов Банка с использованием генеративного ИИ, а также помогает сотрудникам ускорять рабочие процессы (поиск, анализ, документация, разработка кода, тестирование, автоматизация рутины), и все это при соблюдении требований безопасности и комплаенса.
+</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>https://www.postgresql.org/</t>
+  </si>
+  <si>
+    <t>PostgreSQL is a powerful, open source object-relational database system with over 35 years of active development that has earned it a strong reputation for reliability, feature robustness, and performance.</t>
+  </si>
+  <si>
+    <t>Redis</t>
+  </si>
+  <si>
+    <t>mongoDB</t>
+  </si>
+  <si>
+    <t>Apache Kafka</t>
+  </si>
+  <si>
+    <t>auth</t>
+  </si>
+  <si>
+    <t>Zitadel</t>
+  </si>
+  <si>
+    <t>https://confluence.moscow.alfaintra.net/display/PLA/Zitadel</t>
+  </si>
+  <si>
+    <t>ZITADEL is the identity infrastructure platform that is built for developers and works for all users and applications.</t>
+  </si>
+  <si>
+    <t>MongoDB — это популярная NoSQL СУБД, или система управления базами данных, которая предназначена для хранения больших объемов данных в формате документов.</t>
+  </si>
+  <si>
+    <t>https://www.mongodb.com/?version=latest</t>
+  </si>
+  <si>
+    <t>https://redis.io/</t>
+  </si>
+  <si>
+    <t>Redis — нереляционная NoSQL-система управления базами данных (СУБД) с открытым исходным кодом.</t>
+  </si>
+  <si>
+    <t>https://kafka.apache.org/</t>
+  </si>
+  <si>
+    <t>Apache Kafka is an open-source distributed event streaming platform used by thousands of companies for high-performance data pipelines, streaming analytics, data integration</t>
+  </si>
+  <si>
+    <t>Apache Cassandra</t>
+  </si>
+  <si>
+    <t>https://cassandra.apache.org/_/index.html</t>
+  </si>
+  <si>
+    <t>Apache Cassandra is an open source NoSQL distributed database trusted by thousands of companies for scalability and high availability without compromising performance.</t>
+  </si>
+  <si>
+    <t>ElasticSearch</t>
+  </si>
+  <si>
+    <t>https://www.elastic.co/elasticsearch</t>
+  </si>
+  <si>
+    <t>Elasticsearch is the leading distributed, RESTful, open source search and analytics engine designed for speed, horizontal scalability, reliability, and easy management. Get started for free</t>
+  </si>
+  <si>
+    <t>workflow</t>
+  </si>
+  <si>
+    <t>Temporal</t>
+  </si>
+  <si>
+    <t>Temporal — открытая платформа для создания надёжных распределённых приложений. Она решает одну из ключевых проблем современной разработки: как гарантировать выполнение критически важных процессов в нестабильной среде</t>
+  </si>
+  <si>
+    <t>https://temporal.io/</t>
+  </si>
+  <si>
+    <t>Keycloak</t>
+  </si>
+  <si>
+    <t>https://www.keycloak.org/</t>
+  </si>
+  <si>
+    <t>Keycloak provides user federation, strong authentication, user management, fine-grained authorization, and more.</t>
+  </si>
+  <si>
+    <t>BFF</t>
+  </si>
+  <si>
+    <t>https://confluence.moscow.alfaintra.net/pages/viewpage.action?pageId=2769517393</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> архитектурный шаблон, при котором для каждого типа устройства или интерфейса создаётся специальный API-шлюз. Например, можно создать отдельные BFF для браузеров, мобильных приложений или публичных/партнёрских API. </t>
   </si>
 </sst>
 </file>
@@ -450,7 +520,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -473,6 +543,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
@@ -494,11 +565,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D373D6EA-0DEB-453C-A593-8D3D82EAAFD4}" name="Таблица1" displayName="Таблица1" ref="A1:I1048429" totalsRowShown="0" headerRowCellStyle="Акцент1">
-  <autoFilter ref="A1:I1048429" xr:uid="{D373D6EA-0DEB-453C-A593-8D3D82EAAFD4}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I22">
-    <sortCondition ref="A2:A22"/>
-    <sortCondition ref="B2:B22"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D373D6EA-0DEB-453C-A593-8D3D82EAAFD4}" name="Таблица1" displayName="Таблица1" ref="A1:I1048423" totalsRowShown="0" headerRowCellStyle="Акцент1">
+  <autoFilter ref="A1:I1048423" xr:uid="{D373D6EA-0DEB-453C-A593-8D3D82EAAFD4}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I16">
+    <sortCondition ref="A2:A16"/>
+    <sortCondition ref="B2:B16"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{66BF8F95-14AE-4F5F-AF21-8C5AC5095BBF}" name="tags"/>
@@ -832,64 +903,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E083F0B-9B6B-4AE1-B88F-228D13850335}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.5" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="44.28515625" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.5703125" customWidth="1"/>
-    <col min="7" max="7" width="40.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="29.7109375" customWidth="1"/>
-    <col min="9" max="9" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="44.33203125" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
+    <col min="7" max="7" width="40.5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -898,18 +969,18 @@
         <v>6</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -918,18 +989,18 @@
         <v>7</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -938,294 +1009,296 @@
         <v>7</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>51</v>
+      <c r="D5" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>83</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
       <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>81</v>
+        <v>21</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>5</v>
       </c>
       <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
         <v>5</v>
       </c>
       <c r="F10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>101</v>
+        <v>4</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>88</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
         <v>4</v>
       </c>
       <c r="F14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E15" t="s">
         <v>4</v>
       </c>
       <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>85</v>
+      </c>
+      <c r="D17" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F17" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="10" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="G17" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F18" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>29</v>
-      </c>
-      <c r="B18" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E18" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="E19" t="s">
         <v>4</v>
@@ -1233,130 +1306,263 @@
       <c r="F19" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
         <v>83</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" t="s">
         <v>4</v>
       </c>
-      <c r="F20" t="s">
-        <v>8</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="F23" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E24" t="s">
         <v>4</v>
       </c>
-      <c r="F21" t="s">
-        <v>8</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E22" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>72</v>
+      <c r="F24" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" t="s">
+        <v>116</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>119</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E27" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+      <c r="D28" t="s">
+        <v>123</v>
+      </c>
+      <c r="E28" t="s">
+        <v>84</v>
+      </c>
+      <c r="F28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E31" t="s">
+        <v>83</v>
+      </c>
+      <c r="F31" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="D7" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="D6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="D9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="D13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D14" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="D15" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D16" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="D17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="D18" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="D19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
-    <hyperlink ref="D21" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
-    <hyperlink ref="D22" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
-    <hyperlink ref="D10" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
-    <hyperlink ref="D11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
-    <hyperlink ref="D12" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
-    <hyperlink ref="D4" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="D3" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="D20" r:id="rId20" xr:uid="{DD4ACECC-0585-4C8E-B63F-4B8C2C2B9065}"/>
+    <hyperlink ref="D6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="D8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D10" r:id="rId5" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="D11" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="D12" r:id="rId7" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="D13" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="D15" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="D16" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="D4" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="D3" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D14" r:id="rId14" xr:uid="{DD4ACECC-0585-4C8E-B63F-4B8C2C2B9065}"/>
+    <hyperlink ref="D19" r:id="rId15" xr:uid="{06EB6029-C718-824C-93B6-AD4B8D932173}"/>
+    <hyperlink ref="D21" r:id="rId16" xr:uid="{F0078C95-8F44-954D-AAA3-5091A0DFC043}"/>
+    <hyperlink ref="D20" r:id="rId17" xr:uid="{8396D4A7-F089-494F-9098-02E7DFB95112}"/>
+    <hyperlink ref="D26" r:id="rId18" xr:uid="{5403CA65-A7EF-8F46-86C4-19FAF67B5294}"/>
+    <hyperlink ref="D27" r:id="rId19" xr:uid="{D749A71B-E58E-4D4B-A977-51E1E9873834}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId21"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId20"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId21"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{22A5C488-559F-42E7-A17A-04288449D623}">
           <x14:formula1>
             <xm:f>meta!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>F23:F118</xm:sqref>
+          <xm:sqref>F32:F112</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6857320C-10DD-4851-98FA-A3CA686293DC}">
+          <x14:formula1>
+            <xm:f>meta!#REF!</xm:f>
+          </x14:formula1>
+          <xm:sqref>E32:E109</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6E5D21C0-46D9-574F-924F-47FF86B1D17A}">
+          <x14:formula1>
+            <xm:f>quadrants!$A$2:$A$5</xm:f>
+          </x14:formula1>
+          <xm:sqref>E8:E31</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{25C1B5D4-89D9-4337-8B49-80F9A8686BC0}">
+          <x14:formula1>
+            <xm:f>quadrants!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ECCB302B-B329-497F-B6B4-042AE8F9E14B}">
           <x14:formula1>
             <xm:f>meta!$A$2:$A$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I140</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6857320C-10DD-4851-98FA-A3CA686293DC}">
-          <x14:formula1>
-            <xm:f>meta!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E23:E115</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{25C1B5D4-89D9-4337-8B49-80F9A8686BC0}">
-          <x14:formula1>
-            <xm:f>quadrants!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E22</xm:sqref>
+          <xm:sqref>I2:I134</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D7A50CBD-4525-4A5B-95B9-5C2666B34ED9}">
           <x14:formula1>
             <xm:f>rings!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F22</xm:sqref>
+          <xm:sqref>F2:F31</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1369,45 +1575,48 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="103.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="103.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>84</v>
+      </c>
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
     </row>
   </sheetData>
@@ -1421,61 +1630,61 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="86.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="86.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
     </row>
   </sheetData>
@@ -1491,46 +1700,46 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="2" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
fix line sa radar
</commit_message>
<xml_diff>
--- a/public/techRadarSourceSa.xlsx
+++ b/public/techRadarSourceSa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfa/web-alfa/tech-radar/public/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\tech-radar\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97810AA-4432-AF40-8284-65DCEAA141A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633AB0FC-C88A-4F2E-A6F5-D179DF5ED227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2080" yWindow="1400" windowWidth="34560" windowHeight="15720" xr2:uid="{D0E5AF86-51E4-4329-BFCB-5FE4200F8556}"/>
+    <workbookView xWindow="2220" yWindow="1635" windowWidth="31830" windowHeight="12300" xr2:uid="{D0E5AF86-51E4-4329-BFCB-5FE4200F8556}"/>
   </bookViews>
   <sheets>
     <sheet name="radar" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="125">
   <si>
     <t>Ноль</t>
   </si>
@@ -520,7 +520,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
@@ -543,7 +543,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Акцент1" xfId="1" builtinId="29"/>
@@ -903,27 +902,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E083F0B-9B6B-4AE1-B88F-228D13850335}">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" customWidth="1"/>
-    <col min="6" max="6" width="23.5" customWidth="1"/>
-    <col min="7" max="7" width="40.5" style="6" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="44.28515625" customWidth="1"/>
+    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>35</v>
       </c>
@@ -952,7 +951,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -972,7 +971,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -992,7 +991,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1012,7 +1011,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1032,7 +1031,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1052,7 +1051,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1072,7 +1071,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1090,7 +1089,7 @@
       </c>
       <c r="G8" s="11"/>
     </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1110,7 +1109,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1130,7 +1129,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1150,7 +1149,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1170,7 +1169,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -1190,7 +1189,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1210,7 +1209,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -1230,7 +1229,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1250,7 +1249,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1270,7 +1269,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1290,7 +1289,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>92</v>
       </c>
@@ -1310,7 +1309,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>92</v>
       </c>
@@ -1330,7 +1329,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>92</v>
       </c>
@@ -1350,7 +1349,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -1370,7 +1369,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -1390,7 +1389,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
@@ -1410,7 +1409,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>92</v>
       </c>
@@ -1430,7 +1429,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>115</v>
       </c>
@@ -1450,7 +1449,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -1470,7 +1469,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1488,14 +1487,6 @@
       </c>
       <c r="G28" s="6" t="s">
         <v>124</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E31" t="s">
-        <v>83</v>
-      </c>
-      <c r="F31" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1578,13 +1569,13 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5" customWidth="1"/>
-    <col min="2" max="2" width="103.6640625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="103.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>36</v>
       </c>
@@ -1592,31 +1583,31 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="7"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="7"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>83</v>
       </c>
       <c r="B4" s="7"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>84</v>
       </c>
       <c r="B5" s="7"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="9"/>
     </row>
   </sheetData>
@@ -1633,14 +1624,14 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="3" width="86.5" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="86.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>36</v>
       </c>
@@ -1651,7 +1642,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>6</v>
       </c>
@@ -1662,7 +1653,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
@@ -1673,7 +1664,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>8</v>
       </c>
@@ -1684,7 +1675,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
     </row>
   </sheetData>
@@ -1700,12 +1691,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="20.33203125" customWidth="1"/>
+    <col min="1" max="2" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -1713,7 +1704,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1721,7 +1712,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1729,17 +1720,17 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>

</xml_diff>